<commit_message>
Correct plot and code, finish hw2 for KIN 523
</commit_message>
<xml_diff>
--- a/kin523_biomech_mot_activities/hw2/table2.xlsx
+++ b/kin523_biomech_mot_activities/hw2/table2.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyle/MATLAB/osu_coursework/kin523_biomech_mot_activities/hw2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\MATLAB\osu_coursework\kin523_biomech_mot_activities\hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="65120" yWindow="3720" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9750" xr2:uid="{BB5EC348-F204-4DD3-B0F3-C138F37E2C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,25 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="8">
-  <si>
-    <t>Frame</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>delta u</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="2">
   <si>
     <t>&amp;</t>
   </si>
@@ -53,13 +35,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -67,7 +49,7 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -413,1948 +395,1884 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EACAFAF-23AF-433B-8AD4-D29793C3727A}">
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L49" sqref="A1:L49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0.1384</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0.30009999999999998</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0.4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.1862</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0.31640000000000001</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.40360000000000001</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>6.6600000000000006E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.25540000000000002</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.3306</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.41349999999999998</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.34189999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.34050000000000002</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.42930000000000001</v>
+      </c>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.13320000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.43459999999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0.34460000000000002</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.44969999999999999</v>
+      </c>
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>0.1384</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>-0.94620000000000004</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>-0.24249999999999999</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.16650000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.34179999999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.47220000000000001</v>
+      </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>3.3300000000000003E-2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>0.1862</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>-0.92800000000000005</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>-0.23549999999999999</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <f>C3+0.0333</f>
-        <v>6.6600000000000006E-2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>0.25540000000000002</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>-0.90920000000000001</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>-0.22459999999999999</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:C50" si="0">C4+0.0333</f>
-        <v>9.9900000000000017E-2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>0.34189999999999998</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>-0.89229999999999998</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>-0.21049999999999999</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0.13320000000000001</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>0.43459999999999999</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>-0.87980000000000003</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>-0.19470000000000001</v>
-      </c>
-      <c r="J6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0.16650000000000001</v>
+        <v>0.19980000000000001</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.51300000000000001</v>
+        <v>0.5554</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>-0.87370000000000003</v>
+        <v>0.33110000000000001</v>
       </c>
       <c r="H7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>-0.17910000000000001</v>
+        <v>0.49519999999999997</v>
       </c>
       <c r="J7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K7" s="1">
         <v>0.15</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0.19980000000000001</v>
+        <v>0.2331</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.5554</v>
+        <v>0.5454</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-0.87560000000000004</v>
+        <v>0.31230000000000002</v>
       </c>
       <c r="H8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>-0.1653</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="J8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1">
         <v>0.15</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>0.2331</v>
+        <v>0.26640000000000003</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.5454</v>
+        <v>0.48270000000000002</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>-0.88649999999999995</v>
+        <v>0.28620000000000001</v>
       </c>
       <c r="H9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>-0.1552</v>
+        <v>0.53269999999999995</v>
       </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K9" s="1">
         <v>0.15</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0.26640000000000003</v>
+        <v>0.29970000000000002</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0.48270000000000002</v>
+        <v>0.379</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>-0.90610000000000002</v>
+        <v>0.25390000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>-0.15010000000000001</v>
+        <v>0.54259999999999997</v>
       </c>
       <c r="J10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K10" s="1">
         <v>0.15</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0.29970000000000002</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.379</v>
+        <v>0.25790000000000002</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>-0.93379999999999996</v>
+        <v>0.217</v>
       </c>
       <c r="H11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>-0.1515</v>
+        <v>0.54430000000000001</v>
       </c>
       <c r="J11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K11" s="1">
         <v>0.15</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.33300000000000002</v>
+        <v>0.36630000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.25790000000000002</v>
+        <v>0.1462</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>-0.96870000000000001</v>
+        <v>0.17780000000000001</v>
       </c>
       <c r="H12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>-0.16020000000000001</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="J12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1">
         <v>0.15</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0.36630000000000001</v>
+        <v>0.39960000000000001</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.1462</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>-1.0091000000000001</v>
+        <v>0.13869999999999999</v>
       </c>
       <c r="H13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>-0.1769</v>
+        <v>0.51729999999999998</v>
       </c>
       <c r="J13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1">
         <v>0.15</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.39960000000000001</v>
+        <v>0.43290000000000001</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>6.4000000000000001E-2</v>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>-1.0532999999999999</v>
+        <v>0.1024</v>
       </c>
       <c r="H14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>-0.20119999999999999</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="J14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K14" s="1">
         <v>0.15</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0.43290000000000001</v>
+        <v>0.4662</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1.8700000000000001E-2</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>-1.0992999999999999</v>
+        <v>7.2400000000000006E-2</v>
       </c>
       <c r="H15" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>-0.23250000000000001</v>
+        <v>0.44829999999999998</v>
       </c>
       <c r="J15" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K15" s="1">
         <v>0.15</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0.4662</v>
+        <v>0.4995</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>2.0999999999999999E-3</v>
+        <v>-5.7999999999999996E-3</v>
       </c>
       <c r="F16" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>-1.1448</v>
+        <v>5.0299999999999997E-2</v>
       </c>
       <c r="H16" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>-0.26960000000000001</v>
+        <v>0.39979999999999999</v>
       </c>
       <c r="J16" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K16" s="1">
         <v>0.15</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0.4995</v>
+        <v>0.53280000000000005</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>-5.7999999999999996E-3</v>
+        <v>-2.87E-2</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>-1.1883999999999999</v>
+        <v>3.9699999999999999E-2</v>
       </c>
       <c r="H17" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>-0.31080000000000002</v>
+        <v>0.34429999999999999</v>
       </c>
       <c r="J17" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K17" s="1">
         <v>0.15</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>0.53280000000000005</v>
+        <v>0.56610000000000005</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>-2.87E-2</v>
+        <v>-8.3500000000000005E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>-1.2270000000000001</v>
+        <v>4.1399999999999999E-2</v>
       </c>
       <c r="H18" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>-0.3538</v>
+        <v>0.28460000000000002</v>
       </c>
       <c r="J18" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K18" s="1">
         <v>0.15</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>0.56610000000000005</v>
+        <v>0.59940000000000004</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>-8.3500000000000005E-2</v>
+        <v>-0.17050000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>-1.2594000000000001</v>
+        <v>5.7599999999999998E-2</v>
       </c>
       <c r="H19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>-0.39610000000000001</v>
+        <v>0.22339999999999999</v>
       </c>
       <c r="J19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K19" s="1">
         <v>0.15</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>0.59940000000000004</v>
+        <v>0.63270000000000004</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>-0.17050000000000001</v>
+        <v>-0.26719999999999999</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>-1.2824</v>
+        <v>8.8300000000000003E-2</v>
       </c>
       <c r="H20" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>-0.43519999999999998</v>
+        <v>0.1646</v>
       </c>
       <c r="J20" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K20" s="1">
         <v>0.15</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>0.63270000000000004</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>-0.26719999999999999</v>
+        <v>-0.3367</v>
       </c>
       <c r="F21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>-1.2931999999999999</v>
+        <v>0.1333</v>
       </c>
       <c r="H21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>-0.46850000000000003</v>
+        <v>0.11119999999999999</v>
       </c>
       <c r="J21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K21" s="1">
         <v>0.15</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0.66600000000000004</v>
+        <v>0.69930000000000003</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>-0.3367</v>
+        <v>-0.33829999999999999</v>
       </c>
       <c r="F22" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>-1.2884</v>
+        <v>0.19189999999999999</v>
       </c>
       <c r="H22" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>-0.49390000000000001</v>
+        <v>6.7100000000000007E-2</v>
       </c>
       <c r="J22" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K22" s="1">
         <v>0.15</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>0.69930000000000003</v>
+        <v>0.73260000000000003</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>-0.33829999999999999</v>
+        <v>-0.26400000000000001</v>
       </c>
       <c r="F23" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>-1.2634000000000001</v>
+        <v>0.26150000000000001</v>
       </c>
       <c r="H23" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>-0.5091</v>
+        <v>3.5400000000000001E-2</v>
       </c>
       <c r="J23" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K23" s="1">
         <v>0.15</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>0.73260000000000003</v>
+        <v>0.76590000000000003</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>-0.26400000000000001</v>
+        <v>-0.1492</v>
       </c>
       <c r="F24" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>-1.2149000000000001</v>
+        <v>0.3397</v>
       </c>
       <c r="H24" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>-0.51290000000000002</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="J24" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K24" s="1">
         <v>0.15</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>0.76590000000000003</v>
+        <v>0.79920000000000002</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>-0.1492</v>
+        <v>-4.9599999999999998E-2</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>-1.1405000000000001</v>
+        <v>0.42330000000000001</v>
       </c>
       <c r="H25" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>-0.50409999999999999</v>
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="J25" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K25" s="1">
         <v>0.15</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>0.79920000000000002</v>
+        <v>0.83250000000000002</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>-4.9599999999999998E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F26" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>-1.0409999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="H26" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>-0.48180000000000001</v>
+        <v>3.9300000000000002E-2</v>
       </c>
       <c r="J26" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K26" s="1">
         <v>0.15</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
-        <v>0.83250000000000002</v>
+        <v>0.86580000000000001</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>5.5E-2</v>
+        <v>0.3987</v>
       </c>
       <c r="F27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>-0.92220000000000002</v>
+        <v>0.58960000000000001</v>
       </c>
       <c r="H27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>-0.44629999999999997</v>
+        <v>7.8100000000000003E-2</v>
       </c>
       <c r="J27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K27" s="1">
         <v>0.15</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
-        <v>0.86580000000000001</v>
+        <v>0.89910000000000001</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0.3987</v>
+        <v>1.4398</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>-0.79400000000000004</v>
+        <v>0.66379999999999995</v>
       </c>
       <c r="H28" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>-0.3982</v>
+        <v>0.1358</v>
       </c>
       <c r="J28" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K28" s="1">
         <v>0.15</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
-        <v>0.89910000000000001</v>
+        <v>0.93240000000000001</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>1.4398</v>
+        <v>3.5903</v>
       </c>
       <c r="F29" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>-0.66810000000000003</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="H29" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>-0.33879999999999999</v>
+        <v>0.21060000000000001</v>
       </c>
       <c r="J29" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K29" s="1">
         <v>0.15</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
-        <v>0.93240000000000001</v>
+        <v>0.9657</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>3.5903</v>
+        <v>6.8274999999999997</v>
       </c>
       <c r="F30" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>-0.55659999999999998</v>
+        <v>0.77259999999999995</v>
       </c>
       <c r="H30" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>-0.27050000000000002</v>
+        <v>0.2999</v>
       </c>
       <c r="J30" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K30" s="1">
         <v>0.15</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
-        <v>0.9657</v>
+        <v>0.999</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>6.8274999999999997</v>
+        <v>10.5176</v>
       </c>
       <c r="F31" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>-0.46779999999999999</v>
+        <v>0.79990000000000006</v>
       </c>
       <c r="H31" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>-0.1961</v>
+        <v>0.40050000000000002</v>
       </c>
       <c r="J31" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K31" s="1">
         <v>0.15</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
-        <v>0.999</v>
+        <v>1.0323</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>10.5176</v>
+        <v>13.7278</v>
       </c>
       <c r="F32" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>-0.40699999999999997</v>
+        <v>0.8054</v>
       </c>
       <c r="H32" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>-0.1187</v>
+        <v>0.50790000000000002</v>
       </c>
       <c r="J32" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K32" s="1">
         <v>0.15</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
-        <v>1.0323</v>
+        <v>1.0656000000000001</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>13.7278</v>
+        <v>15.6274</v>
       </c>
       <c r="F33" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>-0.37530000000000002</v>
+        <v>0.78720000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>-4.1599999999999998E-2</v>
+        <v>0.61750000000000005</v>
       </c>
       <c r="J33" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K33" s="1">
         <v>0.15</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
-        <v>1.0656000000000001</v>
+        <v>1.0989</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>15.6274</v>
+        <v>15.882400000000001</v>
       </c>
       <c r="F34" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>-0.37290000000000001</v>
+        <v>0.745</v>
       </c>
       <c r="H34" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>3.1699999999999999E-2</v>
+        <v>0.7238</v>
       </c>
       <c r="J34" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K34" s="1">
         <v>0.15</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
-        <v>1.0989000000000002</v>
+        <v>1.1322000000000001</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>15.882400000000001</v>
+        <v>14.6013</v>
       </c>
       <c r="F35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>-0.39729999999999999</v>
+        <v>0.67920000000000003</v>
       </c>
       <c r="H35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>9.7500000000000003E-2</v>
+        <v>0.8216</v>
       </c>
       <c r="J35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K35" s="1">
         <v>0.15</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
-        <v>1.1322000000000003</v>
+        <v>1.1655</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>14.6013</v>
+        <v>12.2286</v>
       </c>
       <c r="F36" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>-0.44619999999999999</v>
+        <v>0.5917</v>
       </c>
       <c r="H36" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>0.1522</v>
+        <v>0.90559999999999996</v>
       </c>
       <c r="J36" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K36" s="1">
         <v>0.15</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
-        <v>1.1655000000000004</v>
+        <v>1.1988000000000001</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>12.2286</v>
+        <v>9.3292000000000002</v>
       </c>
       <c r="F37" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>-0.51659999999999995</v>
+        <v>0.48549999999999999</v>
       </c>
       <c r="H37" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>0.1923</v>
+        <v>0.9708</v>
       </c>
       <c r="J37" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K37" s="1">
         <v>0.15</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
-        <v>1.1988000000000005</v>
+        <v>1.2321</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>9.3292000000000002</v>
+        <v>6.4341999999999997</v>
       </c>
       <c r="F38" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>-0.60489999999999999</v>
+        <v>0.36470000000000002</v>
       </c>
       <c r="H38" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>0.21440000000000001</v>
+        <v>1.0133000000000001</v>
       </c>
       <c r="J38" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K38" s="1">
         <v>0.15</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
-        <v>1.2321000000000006</v>
+        <v>1.2654000000000001</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>6.4341999999999997</v>
+        <v>3.9350000000000001</v>
       </c>
       <c r="F39" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>-0.70760000000000001</v>
+        <v>0.2344</v>
       </c>
       <c r="H39" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>0.2162</v>
+        <v>1.0295000000000001</v>
       </c>
       <c r="J39" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K39" s="1">
         <v>0.15</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
-        <v>1.2654000000000007</v>
+        <v>1.2987</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>3.9350000000000001</v>
+        <v>2.0581999999999998</v>
       </c>
       <c r="F40" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>-0.82030000000000003</v>
+        <v>9.98E-2</v>
       </c>
       <c r="H40" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>0.19570000000000001</v>
+        <v>1.0177</v>
       </c>
       <c r="J40" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K40" s="1">
         <v>0.15</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
-        <v>1.2987000000000009</v>
+        <v>1.3320000000000001</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>2.0581999999999998</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="F41" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>-0.93910000000000005</v>
+        <v>-3.2500000000000001E-2</v>
       </c>
       <c r="H41" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>0.15240000000000001</v>
+        <v>0.97650000000000003</v>
       </c>
       <c r="J41" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K41" s="1">
         <v>0.15</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
-        <v>1.332000000000001</v>
+        <v>1.3653</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>0.86299999999999999</v>
+        <v>0.25919999999999999</v>
       </c>
       <c r="F42" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>-1.0598000000000001</v>
+        <v>-0.156</v>
       </c>
       <c r="H42" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I42">
-        <v>8.6800000000000002E-2</v>
+        <v>0.90680000000000005</v>
       </c>
       <c r="J42" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K42" s="1">
         <v>0.15</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
-        <v>1.3653000000000011</v>
+        <v>1.3986000000000001</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0.25919999999999999</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="F43" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>-1.1780999999999999</v>
+        <v>-0.26469999999999999</v>
       </c>
       <c r="H43" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>1.5E-3</v>
+        <v>0.8105</v>
       </c>
       <c r="J43" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K43" s="1">
         <v>0.15</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
-        <v>1.3986000000000012</v>
+        <v>1.4319</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>2.8799999999999999E-2</v>
+        <v>-0.12759999999999999</v>
       </c>
       <c r="F44" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>-1.2910999999999999</v>
+        <v>-0.35299999999999998</v>
       </c>
       <c r="H44" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>-0.10009999999999999</v>
+        <v>0.69040000000000001</v>
       </c>
       <c r="J44" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K44" s="1">
         <v>0.15</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
-        <v>1.4319000000000013</v>
+        <v>1.4652000000000001</v>
       </c>
       <c r="D45" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>-0.12759999999999999</v>
+        <v>-0.54910000000000003</v>
       </c>
       <c r="F45" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>-1.3975</v>
+        <v>-0.41539999999999999</v>
       </c>
       <c r="H45" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I45">
-        <v>-0.21329999999999999</v>
+        <v>0.55169999999999997</v>
       </c>
       <c r="J45" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K45" s="1">
         <v>0.15</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
-        <v>1.4652000000000014</v>
+        <v>1.4984999999999999</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>-0.54910000000000003</v>
+        <v>-1.5684</v>
       </c>
       <c r="F46" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>-1.4964</v>
+        <v>-0.44819999999999999</v>
       </c>
       <c r="H46" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I46">
-        <v>-0.33179999999999998</v>
+        <v>0.3992</v>
       </c>
       <c r="J46" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K46" s="1">
         <v>0.15</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
-        <v>1.4985000000000015</v>
+        <v>1.5318000000000001</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>-1.5684</v>
+        <v>-3.4418000000000002</v>
       </c>
       <c r="F47" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>-1.5902000000000001</v>
+        <v>-0.44819999999999999</v>
       </c>
       <c r="H47" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>-0.45</v>
+        <v>0.24</v>
       </c>
       <c r="J47" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K47" s="1">
         <v>0.15</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="0"/>
-        <v>1.5318000000000016</v>
+        <v>1.5650999999999999</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>-3.4418000000000002</v>
+        <v>-6.2981999999999996</v>
       </c>
       <c r="F48" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>-1.6819999999999999</v>
+        <v>-0.4143</v>
       </c>
       <c r="H48" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>-0.56100000000000005</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="J48" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K48" s="1">
         <v>0.15</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
-        <v>1.5651000000000017</v>
+        <v>1.5984</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>-6.2981999999999996</v>
+        <v>-10.037699999999999</v>
       </c>
       <c r="F49" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>-1.7768999999999999</v>
+        <v>-0.34660000000000002</v>
       </c>
       <c r="H49" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>-0.65900000000000003</v>
+        <v>-7.0499999999999993E-2</v>
       </c>
       <c r="J49" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K49" s="1">
         <v>0.15</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="0"/>
-        <v>1.5984000000000018</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50">
-        <v>-10.037699999999999</v>
-      </c>
-      <c r="F50" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50">
-        <v>-1.879</v>
-      </c>
-      <c r="H50" t="s">
-        <v>6</v>
-      </c>
-      <c r="I50">
-        <v>-0.73870000000000002</v>
-      </c>
-      <c r="J50" t="s">
-        <v>6</v>
-      </c>
-      <c r="K50" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3:L50" r:id="rId2" display="\\"/>
+    <hyperlink ref="L1" r:id="rId1" xr:uid="{1B36E6C1-FB37-4770-99E6-FF0307381C8A}"/>
+    <hyperlink ref="L2:L49" r:id="rId2" display="\\" xr:uid="{B9A7BB98-AB9C-4EA4-8F8C-B784BC778945}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>